<commit_message>
i think im done
hopefully
</commit_message>
<xml_diff>
--- a/PGI master.xlsx
+++ b/PGI master.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinwininger/Documents/GitHub/PGI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{253263EE-E6E9-6E4E-BEAA-DE2E8A937A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE825FC1-A0D0-6A42-87AB-2443ADABBEEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18060" xr2:uid="{5BADF4EC-349D-7E4C-A00F-F38B4C4743F7}"/>
   </bookViews>
@@ -3788,13 +3788,13 @@
   <dimension ref="A1:S646"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H21" sqref="H21"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="56.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.1640625" customWidth="1"/>
@@ -43190,14 +43190,14 @@
         <v>2140</v>
       </c>
       <c r="F642">
-        <f t="shared" ref="F642:F705" si="50">E642/(D642-J642)</f>
+        <f t="shared" ref="F642:F646" si="50">E642/(D642-J642)</f>
         <v>0.47650857270095748</v>
       </c>
       <c r="G642">
         <v>77</v>
       </c>
       <c r="H642">
-        <f t="shared" ref="H642:H705" si="51">G642/(D642-J642)</f>
+        <f t="shared" ref="H642:H646" si="51">G642/(D642-J642)</f>
         <v>1.7145401914940992E-2</v>
       </c>
       <c r="I642">

</xml_diff>